<commit_message>
Updating packages for github security
</commit_message>
<xml_diff>
--- a/JobImport.xlsx
+++ b/JobImport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\PythonProjects\Django\DjangoJobWebsite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03F852C-1E2B-420B-B772-02D526537344}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1436D29E-9049-4C9B-B209-E893A862D109}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9D9F8F67-FA82-4B81-8CC5-5E6C4A105CAA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>title</t>
   </si>
@@ -54,9 +54,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>2018-03-06</t>
-  </si>
-  <si>
     <t>Imported #1</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
   </si>
   <si>
     <t>OOOh Another one</t>
-  </si>
-  <si>
-    <t>2018-31-12</t>
   </si>
 </sst>
 </file>
@@ -122,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -130,14 +124,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,13 +450,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="24.42578125" style="4" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="6"/>
+    <col min="4" max="4" width="24.42578125" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -477,44 +472,44 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="D2" s="6">
+        <v>43165</v>
+      </c>
+      <c r="E2" s="5">
         <v>10234</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <v>14000</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="D3" s="7">
+        <v>43465</v>
+      </c>
+      <c r="E3" s="5">
         <v>22569</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>45879</v>
       </c>
     </row>

</xml_diff>